<commit_message>
Commit da versão finalizada do trabalho.
</commit_message>
<xml_diff>
--- a/proposicoes_STI_2023.xlsx
+++ b/proposicoes_STI_2023.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B5FBE9-565E-4CD9-B0CC-AC6AC59E1472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44010C8B-B950-428D-8249-61847B28BBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Tratado" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tratado!$A$1:$O$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tratado!$A$1:$K$33</definedName>
     <definedName name="JR_PAGE_ANCHOR_0_1" localSheetId="1">Tratado!#REF!</definedName>
     <definedName name="JR_PAGE_ANCHOR_0_1">Original!#REF!</definedName>
   </definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="84">
   <si>
     <t>Ação Orçamentária</t>
   </si>
@@ -268,12 +268,6 @@
     <t>Unidade Total</t>
   </si>
   <si>
-    <t>SG Limite</t>
-  </si>
-  <si>
-    <t>SG Total</t>
-  </si>
-  <si>
     <t>Gravidade</t>
   </si>
   <si>
@@ -286,24 +280,20 @@
     <t>GUT</t>
   </si>
   <si>
-    <t>SG Extra-Limite</t>
-  </si>
-  <si>
     <t>Manutencao Corretiva/Adaptativa E Sustentacao Softwares</t>
   </si>
   <si>
-    <t>GUT Relativo (GUT/Unidade Total)</t>
+    <t>Soma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00#"/>
-    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,14 +360,6 @@
       <color rgb="FFFF0000"/>
       <name val="SansSerif"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -783,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -954,17 +936,6 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -978,15 +949,9 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1002,15 +967,6 @@
     <xf numFmtId="164" fontId="5" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1020,15 +976,6 @@
     <xf numFmtId="164" fontId="5" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1044,15 +991,6 @@
     <xf numFmtId="164" fontId="5" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1066,20 +1004,14 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1589,23 +1521,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="0.95" customHeight="1" thickBot="1">
-      <c r="A1" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="123" t="s">
+      <c r="A1" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="120"/>
-      <c r="G1" s="123" t="s">
+      <c r="F1" s="104"/>
+      <c r="G1" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="124"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="108"/>
       <c r="L1" s="14"/>
       <c r="M1" s="15"/>
       <c r="N1" s="16"/>
@@ -1614,56 +1546,56 @@
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="121"/>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="126" t="s">
+      <c r="A2" s="105"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="127"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="129" t="s">
+      <c r="M2" s="111"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="130"/>
-      <c r="Q2" s="131"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="115"/>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1">
-      <c r="A3" s="121"/>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="132" t="s">
+      <c r="A3" s="105"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="134" t="s">
+      <c r="M3" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="136" t="s">
+      <c r="N3" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="138" t="s">
+      <c r="O3" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="115" t="s">
+      <c r="P3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="117" t="s">
+      <c r="Q3" s="101" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1679,33 +1611,33 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="137"/>
-      <c r="O4" s="139"/>
-      <c r="P4" s="116"/>
-      <c r="Q4" s="118"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="102"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="101"/>
-      <c r="G5" s="102" t="s">
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="102" t="s">
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="103"/>
+      <c r="K5" s="87"/>
       <c r="L5" s="10">
         <v>7164.3499999999995</v>
       </c>
@@ -1726,19 +1658,19 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="99"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="83"/>
       <c r="L6" s="6">
         <v>7164.3499999999995</v>
       </c>
@@ -1759,25 +1691,25 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="102" t="s">
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="85"/>
+      <c r="G7" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="102" t="s">
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="103"/>
+      <c r="K7" s="87"/>
       <c r="L7" s="10">
         <v>480000</v>
       </c>
@@ -1798,25 +1730,25 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="105"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="106" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="105"/>
-      <c r="G8" s="106" t="s">
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="105"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="106" t="s">
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="107"/>
+      <c r="K8" s="91"/>
       <c r="L8" s="4">
         <v>480000</v>
       </c>
@@ -1837,19 +1769,19 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="99"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="83"/>
       <c r="L9" s="6">
         <v>960000</v>
       </c>
@@ -1870,25 +1802,25 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="30" customHeight="1">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102" t="s">
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="85"/>
+      <c r="G10" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="102" t="s">
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="103"/>
+      <c r="K10" s="87"/>
       <c r="L10" s="10">
         <v>62376.33</v>
       </c>
@@ -1909,19 +1841,19 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="99"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="83"/>
       <c r="L11" s="6">
         <v>62376.33</v>
       </c>
@@ -1942,25 +1874,25 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="101"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="101"/>
-      <c r="G12" s="102" t="s">
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="102" t="s">
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="103"/>
+      <c r="K12" s="87"/>
       <c r="L12" s="10">
         <v>66140.320000000007</v>
       </c>
@@ -1981,19 +1913,19 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="99"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="83"/>
       <c r="L13" s="6">
         <v>66140.320000000007</v>
       </c>
@@ -2014,25 +1946,25 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="101"/>
-      <c r="G14" s="102" t="s">
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="85"/>
+      <c r="G14" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="102" t="s">
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="103"/>
+      <c r="K14" s="87"/>
       <c r="L14" s="10">
         <v>6784</v>
       </c>
@@ -2053,19 +1985,19 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="99"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="83"/>
       <c r="L15" s="6">
         <v>6784</v>
       </c>
@@ -2086,25 +2018,25 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="101"/>
-      <c r="G16" s="102" t="s">
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="85"/>
+      <c r="G16" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="102" t="s">
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="103"/>
+      <c r="K16" s="87"/>
       <c r="L16" s="10">
         <v>176000</v>
       </c>
@@ -2125,19 +2057,19 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="98"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="98"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="99"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="83"/>
       <c r="L17" s="6">
         <v>176000</v>
       </c>
@@ -2158,25 +2090,25 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="30" customHeight="1">
-      <c r="A18" s="100" t="s">
+      <c r="A18" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="101"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="101"/>
-      <c r="G18" s="102" t="s">
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="85"/>
+      <c r="G18" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="102" t="s">
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="103"/>
+      <c r="K18" s="87"/>
       <c r="L18" s="10">
         <v>56000</v>
       </c>
@@ -2197,19 +2129,19 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="98"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="99"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="83"/>
       <c r="L19" s="6">
         <v>56000</v>
       </c>
@@ -2230,25 +2162,25 @@
       </c>
     </row>
     <row r="20" spans="1:17" ht="30" customHeight="1">
-      <c r="A20" s="100" t="s">
+      <c r="A20" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="101"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="102" t="s">
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="101"/>
-      <c r="G20" s="102" t="s">
+      <c r="F20" s="85"/>
+      <c r="G20" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="101"/>
-      <c r="I20" s="101"/>
-      <c r="J20" s="102" t="s">
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="103"/>
+      <c r="K20" s="87"/>
       <c r="L20" s="10">
         <v>671086.16999999993</v>
       </c>
@@ -2269,19 +2201,19 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A21" s="97" t="s">
+      <c r="A21" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="98"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="98"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="99"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="83"/>
       <c r="L21" s="6">
         <v>671086.16999999993</v>
       </c>
@@ -2302,25 +2234,25 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="30" customHeight="1">
-      <c r="A22" s="100" t="s">
+      <c r="A22" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="101"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102" t="s">
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="85"/>
+      <c r="G22" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="101"/>
-      <c r="I22" s="101"/>
-      <c r="J22" s="102" t="s">
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="103"/>
+      <c r="K22" s="87"/>
       <c r="L22" s="10">
         <v>127120.5</v>
       </c>
@@ -2341,19 +2273,19 @@
       </c>
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A23" s="97" t="s">
+      <c r="A23" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23" s="98"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="99"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="83"/>
       <c r="L23" s="6">
         <v>127120.5</v>
       </c>
@@ -2374,25 +2306,25 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="30" customHeight="1">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="101"/>
-      <c r="G24" s="102" t="s">
+      <c r="B24" s="85"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="85"/>
+      <c r="G24" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="101"/>
-      <c r="I24" s="101"/>
-      <c r="J24" s="102" t="s">
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="103"/>
+      <c r="K24" s="87"/>
       <c r="L24" s="10">
         <v>300000</v>
       </c>
@@ -2413,19 +2345,19 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A25" s="97" t="s">
+      <c r="A25" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="98"/>
-      <c r="C25" s="98"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="99"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="83"/>
       <c r="L25" s="6">
         <v>300000</v>
       </c>
@@ -2446,25 +2378,25 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="30" customHeight="1">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="101"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="101"/>
-      <c r="G26" s="102" t="s">
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="85"/>
+      <c r="G26" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
-      <c r="J26" s="102" t="s">
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="103"/>
+      <c r="K26" s="87"/>
       <c r="L26" s="10">
         <v>0</v>
       </c>
@@ -2485,25 +2417,25 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="30" customHeight="1">
-      <c r="A27" s="104" t="s">
+      <c r="A27" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="105"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
-      <c r="E27" s="106" t="s">
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="105"/>
-      <c r="G27" s="106" t="s">
+      <c r="F27" s="89"/>
+      <c r="G27" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="106" t="s">
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="K27" s="107"/>
+      <c r="K27" s="91"/>
       <c r="L27" s="4">
         <v>0</v>
       </c>
@@ -2524,19 +2456,19 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
-      <c r="J28" s="98"/>
-      <c r="K28" s="99"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="83"/>
       <c r="L28" s="6">
         <v>0</v>
       </c>
@@ -2557,25 +2489,25 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="30" customHeight="1">
-      <c r="A29" s="100" t="s">
+      <c r="A29" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="101"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="101"/>
-      <c r="G29" s="102" t="s">
+      <c r="B29" s="85"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="85"/>
+      <c r="G29" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
-      <c r="J29" s="102" t="s">
+      <c r="H29" s="85"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="K29" s="103"/>
+      <c r="K29" s="87"/>
       <c r="L29" s="10">
         <v>154824.32999999999</v>
       </c>
@@ -2596,19 +2528,19 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A30" s="97" t="s">
+      <c r="A30" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="98"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="98"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="98"/>
-      <c r="H30" s="98"/>
-      <c r="I30" s="98"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="99"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="83"/>
       <c r="L30" s="6">
         <v>154824.32999999999</v>
       </c>
@@ -2629,25 +2561,25 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="30" customHeight="1">
-      <c r="A31" s="100" t="s">
+      <c r="A31" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="101"/>
-      <c r="G31" s="102" t="s">
+      <c r="B31" s="85"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="85"/>
+      <c r="G31" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="H31" s="101"/>
-      <c r="I31" s="101"/>
-      <c r="J31" s="102" t="s">
+      <c r="H31" s="85"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="K31" s="103"/>
+      <c r="K31" s="87"/>
       <c r="L31" s="10">
         <v>20000</v>
       </c>
@@ -2668,19 +2600,19 @@
       </c>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="97" t="s">
+      <c r="A32" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="98"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="98"/>
-      <c r="I32" s="98"/>
-      <c r="J32" s="98"/>
-      <c r="K32" s="99"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="83"/>
       <c r="L32" s="6">
         <v>20000</v>
       </c>
@@ -2701,25 +2633,25 @@
       </c>
     </row>
     <row r="33" spans="1:17" ht="30" customHeight="1">
-      <c r="A33" s="100" t="s">
+      <c r="A33" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="101"/>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="101"/>
-      <c r="G33" s="102" t="s">
+      <c r="B33" s="85"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="85"/>
+      <c r="G33" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="H33" s="101"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="102" t="s">
+      <c r="H33" s="85"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K33" s="103"/>
+      <c r="K33" s="87"/>
       <c r="L33" s="10">
         <v>210828.87</v>
       </c>
@@ -2740,19 +2672,19 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A34" s="97" t="s">
+      <c r="A34" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="98"/>
-      <c r="C34" s="98"/>
-      <c r="D34" s="98"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="98"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98"/>
-      <c r="J34" s="98"/>
-      <c r="K34" s="99"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="83"/>
       <c r="L34" s="6">
         <v>210828.87</v>
       </c>
@@ -2773,25 +2705,25 @@
       </c>
     </row>
     <row r="35" spans="1:17" ht="30" customHeight="1">
-      <c r="A35" s="111" t="s">
+      <c r="A35" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="112"/>
-      <c r="C35" s="112"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="113" t="s">
+      <c r="B35" s="96"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="112"/>
-      <c r="G35" s="113" t="s">
+      <c r="F35" s="96"/>
+      <c r="G35" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="H35" s="112"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="113" t="s">
+      <c r="H35" s="96"/>
+      <c r="I35" s="96"/>
+      <c r="J35" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="K35" s="114"/>
+      <c r="K35" s="98"/>
       <c r="L35" s="36">
         <v>376244.72</v>
       </c>
@@ -2812,19 +2744,19 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A36" s="108" t="s">
+      <c r="A36" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="109"/>
-      <c r="C36" s="109"/>
-      <c r="D36" s="109"/>
-      <c r="E36" s="109"/>
-      <c r="F36" s="109"/>
-      <c r="G36" s="109"/>
-      <c r="H36" s="109"/>
-      <c r="I36" s="109"/>
-      <c r="J36" s="109"/>
-      <c r="K36" s="110"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="93"/>
+      <c r="G36" s="93"/>
+      <c r="H36" s="93"/>
+      <c r="I36" s="93"/>
+      <c r="J36" s="93"/>
+      <c r="K36" s="94"/>
       <c r="L36" s="42">
         <v>376244.72</v>
       </c>
@@ -2845,25 +2777,25 @@
       </c>
     </row>
     <row r="37" spans="1:17" ht="30" customHeight="1">
-      <c r="A37" s="100" t="s">
+      <c r="A37" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="101"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="101"/>
-      <c r="G37" s="102" t="s">
+      <c r="B37" s="85"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="85"/>
+      <c r="G37" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="101"/>
-      <c r="I37" s="101"/>
-      <c r="J37" s="102" t="s">
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K37" s="103"/>
+      <c r="K37" s="87"/>
       <c r="L37" s="10">
         <v>50000</v>
       </c>
@@ -2884,19 +2816,19 @@
       </c>
     </row>
     <row r="38" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="98"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="98"/>
-      <c r="G38" s="98"/>
-      <c r="H38" s="98"/>
-      <c r="I38" s="98"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="99"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="83"/>
       <c r="L38" s="6">
         <v>50000</v>
       </c>
@@ -2917,25 +2849,25 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="30" customHeight="1">
-      <c r="A39" s="100" t="s">
+      <c r="A39" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="101"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="101"/>
-      <c r="G39" s="102" t="s">
+      <c r="B39" s="85"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="85"/>
+      <c r="G39" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="101"/>
-      <c r="I39" s="101"/>
-      <c r="J39" s="102" t="s">
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K39" s="103"/>
+      <c r="K39" s="87"/>
       <c r="L39" s="10">
         <v>479808</v>
       </c>
@@ -2956,19 +2888,19 @@
       </c>
     </row>
     <row r="40" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A40" s="97" t="s">
+      <c r="A40" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="98"/>
-      <c r="C40" s="98"/>
-      <c r="D40" s="98"/>
-      <c r="E40" s="98"/>
-      <c r="F40" s="98"/>
-      <c r="G40" s="98"/>
-      <c r="H40" s="98"/>
-      <c r="I40" s="98"/>
-      <c r="J40" s="98"/>
-      <c r="K40" s="99"/>
+      <c r="B40" s="82"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="82"/>
+      <c r="H40" s="82"/>
+      <c r="I40" s="82"/>
+      <c r="J40" s="82"/>
+      <c r="K40" s="83"/>
       <c r="L40" s="6">
         <v>479808</v>
       </c>
@@ -2989,25 +2921,25 @@
       </c>
     </row>
     <row r="41" spans="1:17" ht="28.5" customHeight="1">
-      <c r="A41" s="100" t="s">
+      <c r="A41" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="101"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="101"/>
-      <c r="E41" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="101"/>
-      <c r="G41" s="102" t="s">
+      <c r="B41" s="85"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="85"/>
+      <c r="G41" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="H41" s="101"/>
-      <c r="I41" s="101"/>
-      <c r="J41" s="102" t="s">
+      <c r="H41" s="85"/>
+      <c r="I41" s="85"/>
+      <c r="J41" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="K41" s="103"/>
+      <c r="K41" s="87"/>
       <c r="L41" s="10">
         <v>64800</v>
       </c>
@@ -3028,19 +2960,19 @@
       </c>
     </row>
     <row r="42" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A42" s="97" t="s">
+      <c r="A42" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="98"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="98"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="98"/>
-      <c r="G42" s="98"/>
-      <c r="H42" s="98"/>
-      <c r="I42" s="98"/>
-      <c r="J42" s="98"/>
-      <c r="K42" s="99"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="82"/>
+      <c r="H42" s="82"/>
+      <c r="I42" s="82"/>
+      <c r="J42" s="82"/>
+      <c r="K42" s="83"/>
       <c r="L42" s="6">
         <v>64800</v>
       </c>
@@ -3061,25 +2993,25 @@
       </c>
     </row>
     <row r="43" spans="1:17" ht="30" customHeight="1">
-      <c r="A43" s="100" t="s">
+      <c r="A43" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="101"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="101"/>
-      <c r="E43" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="101"/>
-      <c r="G43" s="102" t="s">
+      <c r="B43" s="85"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="85"/>
+      <c r="G43" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="H43" s="101"/>
-      <c r="I43" s="101"/>
-      <c r="J43" s="102" t="s">
+      <c r="H43" s="85"/>
+      <c r="I43" s="85"/>
+      <c r="J43" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="K43" s="103"/>
+      <c r="K43" s="87"/>
       <c r="L43" s="10">
         <v>532968</v>
       </c>
@@ -3100,19 +3032,19 @@
       </c>
     </row>
     <row r="44" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A44" s="97" t="s">
+      <c r="A44" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="98"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
-      <c r="H44" s="98"/>
-      <c r="I44" s="98"/>
-      <c r="J44" s="98"/>
-      <c r="K44" s="99"/>
+      <c r="B44" s="82"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
+      <c r="G44" s="82"/>
+      <c r="H44" s="82"/>
+      <c r="I44" s="82"/>
+      <c r="J44" s="82"/>
+      <c r="K44" s="83"/>
       <c r="L44" s="6">
         <v>532968</v>
       </c>
@@ -3133,25 +3065,25 @@
       </c>
     </row>
     <row r="45" spans="1:17" ht="30" customHeight="1">
-      <c r="A45" s="100" t="s">
+      <c r="A45" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="101"/>
-      <c r="C45" s="101"/>
-      <c r="D45" s="101"/>
-      <c r="E45" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="101"/>
-      <c r="G45" s="102" t="s">
+      <c r="B45" s="85"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="85"/>
+      <c r="G45" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="H45" s="101"/>
-      <c r="I45" s="101"/>
-      <c r="J45" s="102" t="s">
+      <c r="H45" s="85"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="K45" s="103"/>
+      <c r="K45" s="87"/>
       <c r="L45" s="10">
         <v>413660.94</v>
       </c>
@@ -3172,19 +3104,19 @@
       </c>
     </row>
     <row r="46" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A46" s="97" t="s">
+      <c r="A46" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="98"/>
-      <c r="C46" s="98"/>
-      <c r="D46" s="98"/>
-      <c r="E46" s="98"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="98"/>
-      <c r="I46" s="98"/>
-      <c r="J46" s="98"/>
-      <c r="K46" s="99"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="82"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="82"/>
+      <c r="K46" s="83"/>
       <c r="L46" s="6">
         <v>413660.94</v>
       </c>
@@ -3205,25 +3137,25 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="30" customHeight="1">
-      <c r="A47" s="100" t="s">
+      <c r="A47" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="101"/>
-      <c r="C47" s="101"/>
-      <c r="D47" s="101"/>
-      <c r="E47" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="101"/>
-      <c r="G47" s="102" t="s">
+      <c r="B47" s="85"/>
+      <c r="C47" s="85"/>
+      <c r="D47" s="85"/>
+      <c r="E47" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="85"/>
+      <c r="G47" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="H47" s="101"/>
-      <c r="I47" s="101"/>
-      <c r="J47" s="102" t="s">
+      <c r="H47" s="85"/>
+      <c r="I47" s="85"/>
+      <c r="J47" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="K47" s="103"/>
+      <c r="K47" s="87"/>
       <c r="L47" s="10">
         <v>502208.26</v>
       </c>
@@ -3244,25 +3176,25 @@
       </c>
     </row>
     <row r="48" spans="1:17" ht="30" customHeight="1">
-      <c r="A48" s="104" t="s">
+      <c r="A48" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="105"/>
-      <c r="C48" s="105"/>
-      <c r="D48" s="105"/>
-      <c r="E48" s="106" t="s">
+      <c r="B48" s="89"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="F48" s="105"/>
-      <c r="G48" s="106" t="s">
+      <c r="F48" s="89"/>
+      <c r="G48" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="H48" s="105"/>
-      <c r="I48" s="105"/>
-      <c r="J48" s="106" t="s">
+      <c r="H48" s="89"/>
+      <c r="I48" s="89"/>
+      <c r="J48" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="K48" s="107"/>
+      <c r="K48" s="91"/>
       <c r="L48" s="4">
         <v>1853.42</v>
       </c>
@@ -3283,19 +3215,19 @@
       </c>
     </row>
     <row r="49" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A49" s="97" t="s">
+      <c r="A49" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="98"/>
-      <c r="C49" s="98"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="98"/>
-      <c r="I49" s="98"/>
-      <c r="J49" s="98"/>
-      <c r="K49" s="99"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="82"/>
+      <c r="I49" s="82"/>
+      <c r="J49" s="82"/>
+      <c r="K49" s="83"/>
       <c r="L49" s="6">
         <v>504061.68</v>
       </c>
@@ -3316,25 +3248,25 @@
       </c>
     </row>
     <row r="50" spans="1:17" ht="48" customHeight="1">
-      <c r="A50" s="100" t="s">
+      <c r="A50" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="101"/>
-      <c r="C50" s="101"/>
-      <c r="D50" s="101"/>
-      <c r="E50" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="101"/>
-      <c r="G50" s="102" t="s">
+      <c r="B50" s="85"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="85"/>
+      <c r="G50" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="101"/>
-      <c r="I50" s="101"/>
-      <c r="J50" s="102" t="s">
+      <c r="H50" s="85"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K50" s="103"/>
+      <c r="K50" s="87"/>
       <c r="L50" s="10">
         <v>36883.440000000002</v>
       </c>
@@ -3355,19 +3287,19 @@
       </c>
     </row>
     <row r="51" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A51" s="97" t="s">
+      <c r="A51" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="98"/>
-      <c r="C51" s="98"/>
-      <c r="D51" s="98"/>
-      <c r="E51" s="98"/>
-      <c r="F51" s="98"/>
-      <c r="G51" s="98"/>
-      <c r="H51" s="98"/>
-      <c r="I51" s="98"/>
-      <c r="J51" s="98"/>
-      <c r="K51" s="99"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="82"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="82"/>
+      <c r="H51" s="82"/>
+      <c r="I51" s="82"/>
+      <c r="J51" s="82"/>
+      <c r="K51" s="83"/>
       <c r="L51" s="6">
         <v>36883.440000000002</v>
       </c>
@@ -3388,25 +3320,25 @@
       </c>
     </row>
     <row r="52" spans="1:17" ht="30" customHeight="1">
-      <c r="A52" s="100" t="s">
+      <c r="A52" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="101"/>
-      <c r="C52" s="101"/>
-      <c r="D52" s="101"/>
-      <c r="E52" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="101"/>
-      <c r="G52" s="102" t="s">
+      <c r="B52" s="85"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="85"/>
+      <c r="G52" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H52" s="101"/>
-      <c r="I52" s="101"/>
-      <c r="J52" s="102" t="s">
+      <c r="H52" s="85"/>
+      <c r="I52" s="85"/>
+      <c r="J52" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K52" s="103"/>
+      <c r="K52" s="87"/>
       <c r="L52" s="10">
         <v>7208</v>
       </c>
@@ -3427,19 +3359,19 @@
       </c>
     </row>
     <row r="53" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A53" s="97" t="s">
+      <c r="A53" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="98"/>
-      <c r="C53" s="98"/>
-      <c r="D53" s="98"/>
-      <c r="E53" s="98"/>
-      <c r="F53" s="98"/>
-      <c r="G53" s="98"/>
-      <c r="H53" s="98"/>
-      <c r="I53" s="98"/>
-      <c r="J53" s="98"/>
-      <c r="K53" s="99"/>
+      <c r="B53" s="82"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="82"/>
+      <c r="H53" s="82"/>
+      <c r="I53" s="82"/>
+      <c r="J53" s="82"/>
+      <c r="K53" s="83"/>
       <c r="L53" s="6">
         <v>7208</v>
       </c>
@@ -3460,25 +3392,25 @@
       </c>
     </row>
     <row r="54" spans="1:17" ht="30" customHeight="1">
-      <c r="A54" s="100" t="s">
+      <c r="A54" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="101"/>
-      <c r="C54" s="101"/>
-      <c r="D54" s="101"/>
-      <c r="E54" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="101"/>
-      <c r="G54" s="102" t="s">
+      <c r="B54" s="85"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="85"/>
+      <c r="E54" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="85"/>
+      <c r="G54" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="H54" s="101"/>
-      <c r="I54" s="101"/>
-      <c r="J54" s="102" t="s">
+      <c r="H54" s="85"/>
+      <c r="I54" s="85"/>
+      <c r="J54" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="K54" s="103"/>
+      <c r="K54" s="87"/>
       <c r="L54" s="10">
         <v>38493.050000000003</v>
       </c>
@@ -3499,19 +3431,19 @@
       </c>
     </row>
     <row r="55" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A55" s="97" t="s">
+      <c r="A55" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B55" s="98"/>
-      <c r="C55" s="98"/>
-      <c r="D55" s="98"/>
-      <c r="E55" s="98"/>
-      <c r="F55" s="98"/>
-      <c r="G55" s="98"/>
-      <c r="H55" s="98"/>
-      <c r="I55" s="98"/>
-      <c r="J55" s="98"/>
-      <c r="K55" s="99"/>
+      <c r="B55" s="82"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="82"/>
+      <c r="E55" s="82"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="82"/>
+      <c r="H55" s="82"/>
+      <c r="I55" s="82"/>
+      <c r="J55" s="82"/>
+      <c r="K55" s="83"/>
       <c r="L55" s="6">
         <v>38493.050000000003</v>
       </c>
@@ -3532,25 +3464,25 @@
       </c>
     </row>
     <row r="56" spans="1:17" ht="30" customHeight="1">
-      <c r="A56" s="100" t="s">
+      <c r="A56" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="B56" s="101"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="101"/>
-      <c r="G56" s="102" t="s">
+      <c r="B56" s="85"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="85"/>
+      <c r="G56" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="H56" s="101"/>
-      <c r="I56" s="101"/>
-      <c r="J56" s="102" t="s">
+      <c r="H56" s="85"/>
+      <c r="I56" s="85"/>
+      <c r="J56" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="K56" s="103"/>
+      <c r="K56" s="87"/>
       <c r="L56" s="10">
         <v>80995.94</v>
       </c>
@@ -3571,19 +3503,19 @@
       </c>
     </row>
     <row r="57" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A57" s="97" t="s">
+      <c r="A57" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="98"/>
-      <c r="C57" s="98"/>
-      <c r="D57" s="98"/>
-      <c r="E57" s="98"/>
-      <c r="F57" s="98"/>
-      <c r="G57" s="98"/>
-      <c r="H57" s="98"/>
-      <c r="I57" s="98"/>
-      <c r="J57" s="98"/>
-      <c r="K57" s="99"/>
+      <c r="B57" s="82"/>
+      <c r="C57" s="82"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="82"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="82"/>
+      <c r="I57" s="82"/>
+      <c r="J57" s="82"/>
+      <c r="K57" s="83"/>
       <c r="L57" s="6">
         <v>80995.94</v>
       </c>
@@ -3604,25 +3536,25 @@
       </c>
     </row>
     <row r="58" spans="1:17" ht="30" customHeight="1">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="101"/>
-      <c r="C58" s="101"/>
-      <c r="D58" s="101"/>
-      <c r="E58" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="101"/>
-      <c r="G58" s="102" t="s">
+      <c r="B58" s="85"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="85"/>
+      <c r="G58" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="H58" s="101"/>
-      <c r="I58" s="101"/>
-      <c r="J58" s="102" t="s">
+      <c r="H58" s="85"/>
+      <c r="I58" s="85"/>
+      <c r="J58" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="K58" s="103"/>
+      <c r="K58" s="87"/>
       <c r="L58" s="10">
         <v>103774</v>
       </c>
@@ -3643,19 +3575,19 @@
       </c>
     </row>
     <row r="59" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A59" s="97" t="s">
+      <c r="A59" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="98"/>
-      <c r="C59" s="98"/>
-      <c r="D59" s="98"/>
-      <c r="E59" s="98"/>
-      <c r="F59" s="98"/>
-      <c r="G59" s="98"/>
-      <c r="H59" s="98"/>
-      <c r="I59" s="98"/>
-      <c r="J59" s="98"/>
-      <c r="K59" s="99"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="82"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="83"/>
       <c r="L59" s="6">
         <v>103774</v>
       </c>
@@ -3676,25 +3608,25 @@
       </c>
     </row>
     <row r="60" spans="1:17" ht="30" customHeight="1">
-      <c r="A60" s="100" t="s">
+      <c r="A60" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="101"/>
-      <c r="C60" s="101"/>
-      <c r="D60" s="101"/>
-      <c r="E60" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="101"/>
-      <c r="G60" s="102" t="s">
+      <c r="B60" s="85"/>
+      <c r="C60" s="85"/>
+      <c r="D60" s="85"/>
+      <c r="E60" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="85"/>
+      <c r="G60" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H60" s="101"/>
-      <c r="I60" s="101"/>
-      <c r="J60" s="102" t="s">
+      <c r="H60" s="85"/>
+      <c r="I60" s="85"/>
+      <c r="J60" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="K60" s="103"/>
+      <c r="K60" s="87"/>
       <c r="L60" s="10">
         <v>192349.64</v>
       </c>
@@ -3715,19 +3647,19 @@
       </c>
     </row>
     <row r="61" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A61" s="97" t="s">
+      <c r="A61" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="98"/>
-      <c r="C61" s="98"/>
-      <c r="D61" s="98"/>
-      <c r="E61" s="98"/>
-      <c r="F61" s="98"/>
-      <c r="G61" s="98"/>
-      <c r="H61" s="98"/>
-      <c r="I61" s="98"/>
-      <c r="J61" s="98"/>
-      <c r="K61" s="99"/>
+      <c r="B61" s="82"/>
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+      <c r="E61" s="82"/>
+      <c r="F61" s="82"/>
+      <c r="G61" s="82"/>
+      <c r="H61" s="82"/>
+      <c r="I61" s="82"/>
+      <c r="J61" s="82"/>
+      <c r="K61" s="83"/>
       <c r="L61" s="6">
         <v>192349.64</v>
       </c>
@@ -3748,25 +3680,25 @@
       </c>
     </row>
     <row r="62" spans="1:17" ht="30" customHeight="1">
-      <c r="A62" s="100" t="s">
+      <c r="A62" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="101"/>
-      <c r="C62" s="101"/>
-      <c r="D62" s="101"/>
-      <c r="E62" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="101"/>
-      <c r="G62" s="102" t="s">
+      <c r="B62" s="85"/>
+      <c r="C62" s="85"/>
+      <c r="D62" s="85"/>
+      <c r="E62" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="85"/>
+      <c r="G62" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="H62" s="101"/>
-      <c r="I62" s="101"/>
-      <c r="J62" s="102" t="s">
+      <c r="H62" s="85"/>
+      <c r="I62" s="85"/>
+      <c r="J62" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="K62" s="103"/>
+      <c r="K62" s="87"/>
       <c r="L62" s="10">
         <v>96000</v>
       </c>
@@ -3787,19 +3719,19 @@
       </c>
     </row>
     <row r="63" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A63" s="97" t="s">
+      <c r="A63" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="98"/>
-      <c r="C63" s="98"/>
-      <c r="D63" s="98"/>
-      <c r="E63" s="98"/>
-      <c r="F63" s="98"/>
-      <c r="G63" s="98"/>
-      <c r="H63" s="98"/>
-      <c r="I63" s="98"/>
-      <c r="J63" s="98"/>
-      <c r="K63" s="99"/>
+      <c r="B63" s="82"/>
+      <c r="C63" s="82"/>
+      <c r="D63" s="82"/>
+      <c r="E63" s="82"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="82"/>
+      <c r="H63" s="82"/>
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
+      <c r="K63" s="83"/>
       <c r="L63" s="6">
         <v>96000</v>
       </c>
@@ -3820,25 +3752,25 @@
       </c>
     </row>
     <row r="64" spans="1:17" ht="30" customHeight="1">
-      <c r="A64" s="100" t="s">
+      <c r="A64" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="101"/>
-      <c r="C64" s="101"/>
-      <c r="D64" s="101"/>
-      <c r="E64" s="102" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="101"/>
-      <c r="G64" s="102" t="s">
+      <c r="B64" s="85"/>
+      <c r="C64" s="85"/>
+      <c r="D64" s="85"/>
+      <c r="E64" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="85"/>
+      <c r="G64" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="H64" s="101"/>
-      <c r="I64" s="101"/>
-      <c r="J64" s="102" t="s">
+      <c r="H64" s="85"/>
+      <c r="I64" s="85"/>
+      <c r="J64" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="K64" s="103"/>
+      <c r="K64" s="87"/>
       <c r="L64" s="10">
         <v>404427.72</v>
       </c>
@@ -3859,19 +3791,19 @@
       </c>
     </row>
     <row r="65" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A65" s="97" t="s">
+      <c r="A65" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B65" s="98"/>
-      <c r="C65" s="98"/>
-      <c r="D65" s="98"/>
-      <c r="E65" s="98"/>
-      <c r="F65" s="98"/>
-      <c r="G65" s="98"/>
-      <c r="H65" s="98"/>
-      <c r="I65" s="98"/>
-      <c r="J65" s="98"/>
-      <c r="K65" s="99"/>
+      <c r="B65" s="82"/>
+      <c r="C65" s="82"/>
+      <c r="D65" s="82"/>
+      <c r="E65" s="82"/>
+      <c r="F65" s="82"/>
+      <c r="G65" s="82"/>
+      <c r="H65" s="82"/>
+      <c r="I65" s="82"/>
+      <c r="J65" s="82"/>
+      <c r="K65" s="83"/>
       <c r="L65" s="6">
         <v>404427.72</v>
       </c>
@@ -3892,19 +3824,19 @@
       </c>
     </row>
     <row r="66" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A66" s="94" t="s">
+      <c r="A66" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="95"/>
-      <c r="C66" s="95"/>
-      <c r="D66" s="95"/>
-      <c r="E66" s="95"/>
-      <c r="F66" s="95"/>
-      <c r="G66" s="95"/>
-      <c r="H66" s="95"/>
-      <c r="I66" s="95"/>
-      <c r="J66" s="95"/>
-      <c r="K66" s="96"/>
+      <c r="B66" s="79"/>
+      <c r="C66" s="79"/>
+      <c r="D66" s="79"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="79"/>
+      <c r="G66" s="79"/>
+      <c r="H66" s="79"/>
+      <c r="I66" s="79"/>
+      <c r="J66" s="79"/>
+      <c r="K66" s="80"/>
       <c r="L66" s="17">
         <v>6200000</v>
       </c>
@@ -4125,22 +4057,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="61" customWidth="1"/>
-    <col min="2" max="3" width="15.85546875" style="61"/>
-    <col min="4" max="4" width="40.5703125" style="61" customWidth="1"/>
-    <col min="5" max="8" width="10.5703125" style="61" customWidth="1"/>
-    <col min="9" max="14" width="15.85546875" style="61"/>
-    <col min="15" max="15" width="12.5703125" style="61" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="15.85546875" style="61"/>
+    <col min="1" max="1" width="37.85546875" style="57" customWidth="1"/>
+    <col min="2" max="3" width="15.85546875" style="57" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="57" customWidth="1"/>
+    <col min="5" max="8" width="10.5703125" style="57" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="57"/>
+    <col min="10" max="10" width="15.85546875" style="57" customWidth="1"/>
+    <col min="11" max="16384" width="15.85546875" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="51.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:11" ht="51.75" customHeight="1" thickBot="1">
       <c r="A1" s="47" t="s">
         <v>71</v>
       </c>
@@ -4153,17 +4085,17 @@
       <c r="D1" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="H1" s="53" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>83</v>
       </c>
       <c r="I1" s="50" t="s">
         <v>75</v>
@@ -4174,1669 +4106,1219 @@
       <c r="K1" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="O1" s="60" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A2" s="63" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A2" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="64" t="s">
+      <c r="B2" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="57">
+      <c r="E2" s="54">
         <v>2</v>
       </c>
-      <c r="F2" s="57">
+      <c r="F2" s="54">
         <v>2</v>
       </c>
-      <c r="G2" s="57">
+      <c r="G2" s="54">
         <v>2</v>
       </c>
-      <c r="H2" s="57">
+      <c r="H2" s="54">
         <f t="shared" ref="H2:H33" si="0">E2*F2*G2</f>
         <v>8</v>
       </c>
-      <c r="I2" s="65">
+      <c r="I2" s="60">
         <v>7164.3499999999995</v>
       </c>
-      <c r="J2" s="66">
-        <v>0</v>
-      </c>
-      <c r="K2" s="67">
+      <c r="J2" s="61">
+        <v>0</v>
+      </c>
+      <c r="K2" s="62">
         <f t="shared" ref="K2:K33" si="1">I2+J2</f>
         <v>7164.3499999999995</v>
       </c>
-      <c r="L2" s="68">
-        <v>7164.35</v>
-      </c>
-      <c r="M2" s="69">
-        <v>0</v>
-      </c>
-      <c r="N2" s="70">
-        <f t="shared" ref="N2:N33" si="2">L2+M2</f>
-        <v>7164.35</v>
-      </c>
-      <c r="O2" s="61">
-        <f t="shared" ref="O2:O33" si="3">H2/K2</f>
-        <v>1.116640030149281E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="24">
-      <c r="A3" s="63" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="24">
+      <c r="A3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="64" t="s">
+      <c r="B3" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="57">
+      <c r="E3" s="54">
         <v>3</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="54">
         <v>2</v>
       </c>
-      <c r="G3" s="57">
+      <c r="G3" s="54">
         <v>3</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="54">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I3" s="71">
+      <c r="I3" s="63">
         <v>480000</v>
       </c>
-      <c r="J3" s="72">
-        <v>0</v>
-      </c>
-      <c r="K3" s="73">
+      <c r="J3" s="64">
+        <v>0</v>
+      </c>
+      <c r="K3" s="65">
         <f t="shared" si="1"/>
         <v>480000</v>
       </c>
-      <c r="L3" s="74">
-        <v>480000</v>
-      </c>
-      <c r="M3" s="75">
-        <v>0</v>
-      </c>
-      <c r="N3" s="76">
-        <f t="shared" si="2"/>
-        <v>480000</v>
-      </c>
-      <c r="O3" s="61">
-        <f t="shared" si="3"/>
-        <v>3.7499999999999997E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="24.75" thickBot="1">
-      <c r="A4" s="77" t="s">
+    </row>
+    <row r="4" spans="1:11" ht="24.75" thickBot="1">
+      <c r="A4" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="78" t="s">
+      <c r="B4" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="55">
         <v>3</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="55">
         <v>2</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="55">
         <v>3</v>
       </c>
-      <c r="H4" s="58">
+      <c r="H4" s="55">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I4" s="79">
+      <c r="I4" s="68">
         <v>480000</v>
       </c>
-      <c r="J4" s="80">
-        <v>0</v>
-      </c>
-      <c r="K4" s="81">
+      <c r="J4" s="69">
+        <v>0</v>
+      </c>
+      <c r="K4" s="70">
         <f t="shared" si="1"/>
         <v>480000</v>
       </c>
-      <c r="L4" s="82">
-        <v>480000</v>
-      </c>
-      <c r="M4" s="83">
-        <v>0</v>
-      </c>
-      <c r="N4" s="84">
-        <f t="shared" si="2"/>
-        <v>480000</v>
-      </c>
-      <c r="O4" s="61">
-        <f t="shared" si="3"/>
-        <v>3.7499999999999997E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A5" s="63" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A5" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="57">
+      <c r="E5" s="54">
         <v>5</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="54">
         <v>5</v>
       </c>
-      <c r="G5" s="57">
+      <c r="G5" s="54">
         <v>5</v>
       </c>
-      <c r="H5" s="57">
+      <c r="H5" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I5" s="71">
+      <c r="I5" s="63">
         <v>62376.33</v>
       </c>
-      <c r="J5" s="72">
-        <v>0</v>
-      </c>
-      <c r="K5" s="73">
+      <c r="J5" s="64">
+        <v>0</v>
+      </c>
+      <c r="K5" s="65">
         <f t="shared" si="1"/>
         <v>62376.33</v>
       </c>
-      <c r="L5" s="74">
-        <v>62376.33</v>
-      </c>
-      <c r="M5" s="75">
-        <v>0</v>
-      </c>
-      <c r="N5" s="76">
-        <f t="shared" si="2"/>
-        <v>62376.33</v>
-      </c>
-      <c r="O5" s="61">
-        <f t="shared" si="3"/>
-        <v>2.003965286191092E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A6" s="63" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A6" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="64" t="s">
+      <c r="B6" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="57">
+      <c r="E6" s="54">
         <v>5</v>
       </c>
-      <c r="F6" s="57">
+      <c r="F6" s="54">
         <v>5</v>
       </c>
-      <c r="G6" s="57">
+      <c r="G6" s="54">
         <v>5</v>
       </c>
-      <c r="H6" s="57">
+      <c r="H6" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I6" s="71">
+      <c r="I6" s="63">
         <v>66140.320000000007</v>
       </c>
-      <c r="J6" s="72">
-        <v>0</v>
-      </c>
-      <c r="K6" s="73">
+      <c r="J6" s="64">
+        <v>0</v>
+      </c>
+      <c r="K6" s="65">
         <f t="shared" si="1"/>
         <v>66140.320000000007</v>
       </c>
-      <c r="L6" s="74">
-        <v>66140.320000000007</v>
-      </c>
-      <c r="M6" s="75">
-        <v>0</v>
-      </c>
-      <c r="N6" s="76">
-        <f t="shared" si="2"/>
-        <v>66140.320000000007</v>
-      </c>
-      <c r="O6" s="61">
-        <f t="shared" si="3"/>
-        <v>1.8899213067006628E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A7" s="63" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A7" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="64" t="s">
+      <c r="B7" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="57">
+      <c r="E7" s="54">
         <v>5</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="54">
         <v>3</v>
       </c>
-      <c r="G7" s="57">
+      <c r="G7" s="54">
         <v>3</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="54">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="I7" s="71">
+      <c r="I7" s="63">
         <v>6784</v>
       </c>
-      <c r="J7" s="72">
-        <v>0</v>
-      </c>
-      <c r="K7" s="73">
+      <c r="J7" s="64">
+        <v>0</v>
+      </c>
+      <c r="K7" s="65">
         <f t="shared" si="1"/>
         <v>6784</v>
       </c>
-      <c r="L7" s="74">
-        <v>6784</v>
-      </c>
-      <c r="M7" s="75">
-        <v>0</v>
-      </c>
-      <c r="N7" s="76">
-        <f t="shared" si="2"/>
-        <v>6784</v>
-      </c>
-      <c r="O7" s="61">
-        <f t="shared" si="3"/>
-        <v>6.6332547169811323E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A8" s="63" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A8" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="64" t="s">
+      <c r="B8" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="57">
+      <c r="E8" s="54">
         <v>2</v>
       </c>
-      <c r="F8" s="57">
+      <c r="F8" s="54">
         <v>2</v>
       </c>
-      <c r="G8" s="57">
+      <c r="G8" s="54">
         <v>4</v>
       </c>
-      <c r="H8" s="57">
+      <c r="H8" s="54">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I8" s="71">
+      <c r="I8" s="63">
         <v>176000</v>
       </c>
-      <c r="J8" s="72">
-        <v>0</v>
-      </c>
-      <c r="K8" s="73">
+      <c r="J8" s="64">
+        <v>0</v>
+      </c>
+      <c r="K8" s="65">
         <f t="shared" si="1"/>
         <v>176000</v>
       </c>
-      <c r="L8" s="74">
-        <v>176000</v>
-      </c>
-      <c r="M8" s="75">
-        <v>0</v>
-      </c>
-      <c r="N8" s="76">
-        <f t="shared" si="2"/>
-        <v>176000</v>
-      </c>
-      <c r="O8" s="61">
-        <f t="shared" si="3"/>
-        <v>9.0909090909090904E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A9" s="63" t="s">
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A9" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="64" t="s">
+      <c r="B9" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="57">
+      <c r="E9" s="54">
         <v>2</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="54">
         <v>2</v>
       </c>
-      <c r="G9" s="57">
+      <c r="G9" s="54">
         <v>4</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="54">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I9" s="71">
+      <c r="I9" s="63">
         <v>56000</v>
       </c>
-      <c r="J9" s="72">
-        <v>0</v>
-      </c>
-      <c r="K9" s="73">
+      <c r="J9" s="64">
+        <v>0</v>
+      </c>
+      <c r="K9" s="65">
         <f t="shared" si="1"/>
         <v>56000</v>
       </c>
-      <c r="L9" s="74">
-        <v>56000</v>
-      </c>
-      <c r="M9" s="75">
-        <v>0</v>
-      </c>
-      <c r="N9" s="76">
-        <f t="shared" si="2"/>
-        <v>56000</v>
-      </c>
-      <c r="O9" s="61">
-        <f t="shared" si="3"/>
-        <v>2.8571428571428574E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A10" s="63" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A10" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="57">
+      <c r="E10" s="54">
         <v>5</v>
       </c>
-      <c r="F10" s="57">
+      <c r="F10" s="54">
         <v>3</v>
       </c>
-      <c r="G10" s="57">
+      <c r="G10" s="54">
         <v>5</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="54">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="I10" s="71">
+      <c r="I10" s="63">
         <v>671086.16999999993</v>
       </c>
-      <c r="J10" s="72">
-        <v>0</v>
-      </c>
-      <c r="K10" s="73">
+      <c r="J10" s="64">
+        <v>0</v>
+      </c>
+      <c r="K10" s="65">
         <f t="shared" si="1"/>
         <v>671086.16999999993</v>
       </c>
-      <c r="L10" s="74">
-        <v>671086.17000000004</v>
-      </c>
-      <c r="M10" s="75">
-        <v>0</v>
-      </c>
-      <c r="N10" s="76">
-        <f t="shared" si="2"/>
-        <v>671086.17000000004</v>
-      </c>
-      <c r="O10" s="61">
-        <f t="shared" si="3"/>
-        <v>1.1175912029300203E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A11" s="63" t="s">
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A11" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="64" t="s">
+      <c r="B11" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="54">
         <v>4</v>
       </c>
-      <c r="F11" s="57">
+      <c r="F11" s="54">
         <v>4</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="54">
         <v>5</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="54">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="I11" s="71">
+      <c r="I11" s="63">
         <v>127120.5</v>
       </c>
-      <c r="J11" s="72">
-        <v>0</v>
-      </c>
-      <c r="K11" s="73">
+      <c r="J11" s="64">
+        <v>0</v>
+      </c>
+      <c r="K11" s="65">
         <f t="shared" si="1"/>
         <v>127120.5</v>
       </c>
-      <c r="L11" s="74">
-        <v>127120.5</v>
-      </c>
-      <c r="M11" s="75">
-        <v>0</v>
-      </c>
-      <c r="N11" s="76">
-        <f t="shared" si="2"/>
-        <v>127120.5</v>
-      </c>
-      <c r="O11" s="61">
-        <f t="shared" si="3"/>
-        <v>6.293241452008134E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A12" s="63" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A12" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="64" t="s">
+      <c r="B12" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="57">
+      <c r="E12" s="54">
         <v>2</v>
       </c>
-      <c r="F12" s="57">
+      <c r="F12" s="54">
         <v>3</v>
       </c>
-      <c r="G12" s="57">
+      <c r="G12" s="54">
         <v>3</v>
       </c>
-      <c r="H12" s="57">
+      <c r="H12" s="54">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I12" s="71">
+      <c r="I12" s="63">
         <v>300000</v>
       </c>
-      <c r="J12" s="72">
-        <v>0</v>
-      </c>
-      <c r="K12" s="73">
+      <c r="J12" s="64">
+        <v>0</v>
+      </c>
+      <c r="K12" s="65">
         <f t="shared" si="1"/>
         <v>300000</v>
       </c>
-      <c r="L12" s="74">
-        <v>300000</v>
-      </c>
-      <c r="M12" s="75">
-        <v>0</v>
-      </c>
-      <c r="N12" s="76">
-        <f t="shared" si="2"/>
-        <v>300000</v>
-      </c>
-      <c r="O12" s="61">
-        <f t="shared" si="3"/>
-        <v>6.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="30" customHeight="1">
-      <c r="A13" s="63" t="s">
+    </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1">
+      <c r="A13" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="64" t="s">
+      <c r="B13" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="57">
+      <c r="E13" s="54">
         <v>3</v>
       </c>
-      <c r="F13" s="57">
+      <c r="F13" s="54">
         <v>3</v>
       </c>
-      <c r="G13" s="57">
+      <c r="G13" s="54">
         <v>3</v>
       </c>
-      <c r="H13" s="57">
+      <c r="H13" s="54">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="I13" s="71">
-        <v>0</v>
-      </c>
-      <c r="J13" s="72">
+      <c r="I13" s="63">
+        <v>0</v>
+      </c>
+      <c r="J13" s="64">
         <v>75900</v>
       </c>
-      <c r="K13" s="73">
+      <c r="K13" s="65">
         <f t="shared" si="1"/>
         <v>75900</v>
       </c>
-      <c r="L13" s="74">
-        <v>0</v>
-      </c>
-      <c r="M13" s="75">
-        <v>75900</v>
-      </c>
-      <c r="N13" s="76">
-        <f t="shared" si="2"/>
-        <v>75900</v>
-      </c>
-      <c r="O13" s="61">
-        <f t="shared" si="3"/>
-        <v>3.5573122529644266E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="77" t="s">
+    </row>
+    <row r="14" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A14" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="78" t="s">
+      <c r="D14" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="58">
+      <c r="E14" s="55">
         <v>3</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="55">
         <v>3</v>
       </c>
-      <c r="G14" s="58">
+      <c r="G14" s="55">
         <v>3</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="55">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="I14" s="79">
-        <v>0</v>
-      </c>
-      <c r="J14" s="80">
+      <c r="I14" s="68">
+        <v>0</v>
+      </c>
+      <c r="J14" s="69">
         <v>346500</v>
       </c>
-      <c r="K14" s="81">
+      <c r="K14" s="70">
         <f t="shared" si="1"/>
         <v>346500</v>
       </c>
-      <c r="L14" s="82">
-        <v>0</v>
-      </c>
-      <c r="M14" s="83">
-        <v>346500</v>
-      </c>
-      <c r="N14" s="84">
-        <f t="shared" si="2"/>
-        <v>346500</v>
-      </c>
-      <c r="O14" s="61">
-        <f t="shared" si="3"/>
-        <v>7.7922077922077919E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A15" s="63" t="s">
+    </row>
+    <row r="15" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A15" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="64" t="s">
+      <c r="B15" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="57">
+      <c r="E15" s="54">
         <v>5</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F15" s="54">
         <v>5</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G15" s="54">
         <v>5</v>
       </c>
-      <c r="H15" s="57">
+      <c r="H15" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I15" s="71">
+      <c r="I15" s="63">
         <v>154824.32999999999</v>
       </c>
-      <c r="J15" s="72">
-        <v>0</v>
-      </c>
-      <c r="K15" s="73">
+      <c r="J15" s="64">
+        <v>0</v>
+      </c>
+      <c r="K15" s="65">
         <f t="shared" si="1"/>
         <v>154824.32999999999</v>
       </c>
-      <c r="L15" s="74">
-        <v>154824.32999999999</v>
-      </c>
-      <c r="M15" s="75">
-        <v>0</v>
-      </c>
-      <c r="N15" s="76">
-        <f t="shared" si="2"/>
-        <v>154824.32999999999</v>
-      </c>
-      <c r="O15" s="61">
-        <f t="shared" si="3"/>
-        <v>8.0736664579785368E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A16" s="63" t="s">
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A16" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="57">
+      <c r="E16" s="54">
         <v>1</v>
       </c>
-      <c r="F16" s="57">
+      <c r="F16" s="54">
         <v>1</v>
       </c>
-      <c r="G16" s="57">
+      <c r="G16" s="54">
         <v>1</v>
       </c>
-      <c r="H16" s="57">
+      <c r="H16" s="54">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I16" s="71">
+      <c r="I16" s="63">
         <v>20000</v>
       </c>
-      <c r="J16" s="72">
-        <v>0</v>
-      </c>
-      <c r="K16" s="73">
+      <c r="J16" s="64">
+        <v>0</v>
+      </c>
+      <c r="K16" s="65">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
-      <c r="L16" s="74">
-        <v>20000</v>
-      </c>
-      <c r="M16" s="75">
-        <v>0</v>
-      </c>
-      <c r="N16" s="76">
-        <f t="shared" si="2"/>
-        <v>20000</v>
-      </c>
-      <c r="O16" s="61">
-        <f t="shared" si="3"/>
-        <v>5.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A17" s="63" t="s">
+    </row>
+    <row r="17" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A17" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="64" t="s">
+      <c r="B17" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="57">
+      <c r="E17" s="54">
         <v>4</v>
       </c>
-      <c r="F17" s="57">
+      <c r="F17" s="54">
         <v>5</v>
       </c>
-      <c r="G17" s="57">
+      <c r="G17" s="54">
         <v>5</v>
       </c>
-      <c r="H17" s="57">
+      <c r="H17" s="54">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="I17" s="71">
+      <c r="I17" s="63">
         <v>210828.87</v>
       </c>
-      <c r="J17" s="72">
-        <v>0</v>
-      </c>
-      <c r="K17" s="73">
+      <c r="J17" s="64">
+        <v>0</v>
+      </c>
+      <c r="K17" s="65">
         <f t="shared" si="1"/>
         <v>210828.87</v>
       </c>
-      <c r="L17" s="74">
-        <v>210828.87</v>
-      </c>
-      <c r="M17" s="75">
-        <v>0</v>
-      </c>
-      <c r="N17" s="76">
-        <f t="shared" si="2"/>
-        <v>210828.87</v>
-      </c>
-      <c r="O17" s="61">
-        <f t="shared" si="3"/>
-        <v>4.7431834169580289E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A18" s="85" t="s">
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A18" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="59">
+      <c r="E18" s="56">
         <v>3</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F18" s="56">
         <v>3</v>
       </c>
-      <c r="G18" s="59">
+      <c r="G18" s="56">
         <v>5</v>
       </c>
-      <c r="H18" s="59">
+      <c r="H18" s="56">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="I18" s="87">
-        <v>376244.72</v>
-      </c>
-      <c r="J18" s="88">
-        <v>1023755.28</v>
-      </c>
-      <c r="K18" s="89">
+      <c r="I18" s="73">
+        <v>0</v>
+      </c>
+      <c r="J18" s="74">
+        <v>1400000</v>
+      </c>
+      <c r="K18" s="75">
         <f t="shared" si="1"/>
         <v>1400000</v>
       </c>
-      <c r="L18" s="90">
-        <v>376244.72</v>
-      </c>
-      <c r="M18" s="91">
-        <v>0</v>
-      </c>
-      <c r="N18" s="92">
-        <f t="shared" si="2"/>
-        <v>376244.72</v>
-      </c>
-      <c r="O18" s="61">
-        <f t="shared" si="3"/>
-        <v>3.2142857142857144E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A19" s="63" t="s">
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A19" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="64" t="s">
+      <c r="B19" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="57">
+      <c r="E19" s="54">
         <v>1</v>
       </c>
-      <c r="F19" s="57">
+      <c r="F19" s="54">
         <v>1</v>
       </c>
-      <c r="G19" s="57">
+      <c r="G19" s="54">
         <v>1</v>
       </c>
-      <c r="H19" s="57">
+      <c r="H19" s="54">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I19" s="71">
+      <c r="I19" s="63">
         <v>50000</v>
       </c>
-      <c r="J19" s="72">
-        <v>0</v>
-      </c>
-      <c r="K19" s="73">
+      <c r="J19" s="64">
+        <v>0</v>
+      </c>
+      <c r="K19" s="65">
         <f t="shared" si="1"/>
         <v>50000</v>
       </c>
-      <c r="L19" s="74">
-        <v>50000</v>
-      </c>
-      <c r="M19" s="75">
-        <v>0</v>
-      </c>
-      <c r="N19" s="76">
-        <f t="shared" si="2"/>
-        <v>50000</v>
-      </c>
-      <c r="O19" s="61">
-        <f t="shared" si="3"/>
-        <v>2.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A20" s="63" t="s">
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A20" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="57">
+      <c r="E20" s="54">
         <v>5</v>
       </c>
-      <c r="F20" s="57">
+      <c r="F20" s="54">
         <v>5</v>
       </c>
-      <c r="G20" s="57">
+      <c r="G20" s="54">
         <v>5</v>
       </c>
-      <c r="H20" s="57">
+      <c r="H20" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I20" s="71">
+      <c r="I20" s="63">
         <v>479808</v>
       </c>
-      <c r="J20" s="72">
-        <v>0</v>
-      </c>
-      <c r="K20" s="73">
+      <c r="J20" s="64">
+        <v>0</v>
+      </c>
+      <c r="K20" s="65">
         <f t="shared" si="1"/>
         <v>479808</v>
       </c>
-      <c r="L20" s="74">
-        <v>479808</v>
-      </c>
-      <c r="M20" s="75">
-        <v>0</v>
-      </c>
-      <c r="N20" s="76">
-        <f t="shared" si="2"/>
-        <v>479808</v>
-      </c>
-      <c r="O20" s="61">
-        <f t="shared" si="3"/>
-        <v>2.6052087501667336E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A21" s="63" t="s">
+    </row>
+    <row r="21" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A21" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="64" t="s">
+      <c r="B21" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="57">
+      <c r="D21" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="54">
         <v>5</v>
       </c>
-      <c r="F21" s="57">
+      <c r="F21" s="54">
         <v>4</v>
       </c>
-      <c r="G21" s="57">
+      <c r="G21" s="54">
         <v>4</v>
       </c>
-      <c r="H21" s="57">
+      <c r="H21" s="54">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="I21" s="71">
+      <c r="I21" s="63">
         <v>64800</v>
       </c>
-      <c r="J21" s="72">
-        <v>0</v>
-      </c>
-      <c r="K21" s="73">
+      <c r="J21" s="64">
+        <v>0</v>
+      </c>
+      <c r="K21" s="65">
         <f t="shared" si="1"/>
         <v>64800</v>
       </c>
-      <c r="L21" s="74">
-        <v>64800</v>
-      </c>
-      <c r="M21" s="75">
-        <v>0</v>
-      </c>
-      <c r="N21" s="76">
-        <f t="shared" si="2"/>
-        <v>64800</v>
-      </c>
-      <c r="O21" s="61">
-        <f t="shared" si="3"/>
-        <v>1.2345679012345679E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A22" s="63" t="s">
+    </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A22" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="64" t="s">
+      <c r="D22" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="57">
+      <c r="E22" s="54">
         <v>1</v>
       </c>
-      <c r="F22" s="57">
+      <c r="F22" s="54">
         <v>1</v>
       </c>
-      <c r="G22" s="57">
+      <c r="G22" s="54">
         <v>1</v>
       </c>
-      <c r="H22" s="57">
+      <c r="H22" s="54">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I22" s="71">
+      <c r="I22" s="63">
         <v>532968</v>
       </c>
-      <c r="J22" s="72">
-        <v>0</v>
-      </c>
-      <c r="K22" s="73">
+      <c r="J22" s="64">
+        <v>0</v>
+      </c>
+      <c r="K22" s="65">
         <f t="shared" si="1"/>
         <v>532968</v>
       </c>
-      <c r="L22" s="74">
-        <v>532968</v>
-      </c>
-      <c r="M22" s="75">
-        <v>0</v>
-      </c>
-      <c r="N22" s="76">
-        <f t="shared" si="2"/>
-        <v>532968</v>
-      </c>
-      <c r="O22" s="62">
-        <f t="shared" si="3"/>
-        <v>1.876285255399949E-6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A23" s="63" t="s">
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A23" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="64" t="s">
+      <c r="B23" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="64" t="s">
+      <c r="D23" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="57">
+      <c r="E23" s="54">
         <v>5</v>
       </c>
-      <c r="F23" s="57">
+      <c r="F23" s="54">
         <v>5</v>
       </c>
-      <c r="G23" s="57">
+      <c r="G23" s="54">
         <v>5</v>
       </c>
-      <c r="H23" s="57">
+      <c r="H23" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I23" s="71">
+      <c r="I23" s="63">
         <v>413660.94</v>
       </c>
-      <c r="J23" s="72">
-        <v>0</v>
-      </c>
-      <c r="K23" s="73">
+      <c r="J23" s="64">
+        <v>0</v>
+      </c>
+      <c r="K23" s="65">
         <f t="shared" si="1"/>
         <v>413660.94</v>
       </c>
-      <c r="L23" s="74">
-        <v>413660.94</v>
-      </c>
-      <c r="M23" s="75">
-        <v>0</v>
-      </c>
-      <c r="N23" s="76">
-        <f t="shared" si="2"/>
-        <v>413660.94</v>
-      </c>
-      <c r="O23" s="61">
-        <f t="shared" si="3"/>
-        <v>3.0217984806590637E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="30" customHeight="1">
-      <c r="A24" s="63" t="s">
+    </row>
+    <row r="24" spans="1:11" ht="30" customHeight="1">
+      <c r="A24" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="64" t="s">
+      <c r="B24" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="64" t="s">
+      <c r="D24" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="57">
+      <c r="E24" s="54">
         <v>2</v>
       </c>
-      <c r="F24" s="57">
+      <c r="F24" s="54">
         <v>2</v>
       </c>
-      <c r="G24" s="57">
+      <c r="G24" s="54">
         <v>2</v>
       </c>
-      <c r="H24" s="57">
+      <c r="H24" s="54">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I24" s="71">
+      <c r="I24" s="63">
         <v>36883.440000000002</v>
       </c>
-      <c r="J24" s="72">
-        <v>0</v>
-      </c>
-      <c r="K24" s="73">
+      <c r="J24" s="64">
+        <v>0</v>
+      </c>
+      <c r="K24" s="65">
         <f t="shared" si="1"/>
         <v>36883.440000000002</v>
       </c>
-      <c r="L24" s="74">
-        <v>36883.440000000002</v>
-      </c>
-      <c r="M24" s="75">
-        <v>0</v>
-      </c>
-      <c r="N24" s="76">
-        <f t="shared" si="2"/>
-        <v>36883.440000000002</v>
-      </c>
-      <c r="O24" s="61">
-        <f t="shared" si="3"/>
-        <v>2.1689950828881471E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A25" s="77" t="s">
+    </row>
+    <row r="25" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A25" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="78" t="s">
+      <c r="B25" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="78" t="s">
+      <c r="D25" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="58">
+      <c r="E25" s="55">
         <v>5</v>
       </c>
-      <c r="F25" s="58">
+      <c r="F25" s="55">
         <v>5</v>
       </c>
-      <c r="G25" s="58">
+      <c r="G25" s="55">
         <v>5</v>
       </c>
-      <c r="H25" s="58">
+      <c r="H25" s="55">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I25" s="79">
+      <c r="I25" s="68">
         <v>7208</v>
       </c>
-      <c r="J25" s="80">
-        <v>0</v>
-      </c>
-      <c r="K25" s="81">
+      <c r="J25" s="69">
+        <v>0</v>
+      </c>
+      <c r="K25" s="70">
         <f t="shared" si="1"/>
         <v>7208</v>
       </c>
-      <c r="L25" s="82">
-        <v>7208</v>
-      </c>
-      <c r="M25" s="83">
-        <v>0</v>
-      </c>
-      <c r="N25" s="84">
-        <f t="shared" si="2"/>
-        <v>7208</v>
-      </c>
-      <c r="O25" s="61">
-        <f t="shared" si="3"/>
-        <v>1.7341842397336292E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="48" customHeight="1" thickBot="1">
-      <c r="A26" s="63" t="s">
+    </row>
+    <row r="26" spans="1:11" ht="48" customHeight="1" thickBot="1">
+      <c r="A26" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="64" t="s">
+      <c r="B26" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="57">
+      <c r="D26" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="54">
         <v>5</v>
       </c>
-      <c r="F26" s="57">
+      <c r="F26" s="54">
         <v>5</v>
       </c>
-      <c r="G26" s="57">
+      <c r="G26" s="54">
         <v>5</v>
       </c>
-      <c r="H26" s="57">
+      <c r="H26" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I26" s="71">
+      <c r="I26" s="63">
         <v>38493.050000000003</v>
       </c>
-      <c r="J26" s="72">
-        <v>0</v>
-      </c>
-      <c r="K26" s="73">
+      <c r="J26" s="64">
+        <v>0</v>
+      </c>
+      <c r="K26" s="65">
         <f t="shared" si="1"/>
         <v>38493.050000000003</v>
       </c>
-      <c r="L26" s="74">
-        <v>38493.050000000003</v>
-      </c>
-      <c r="M26" s="75">
-        <v>0</v>
-      </c>
-      <c r="N26" s="76">
-        <f t="shared" si="2"/>
-        <v>38493.050000000003</v>
-      </c>
-      <c r="O26" s="61">
-        <f t="shared" si="3"/>
-        <v>3.2473394547846948E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A27" s="63" t="s">
+    </row>
+    <row r="27" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A27" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="57">
+      <c r="D27" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="54">
         <v>5</v>
       </c>
-      <c r="F27" s="57">
+      <c r="F27" s="54">
         <v>5</v>
       </c>
-      <c r="G27" s="57">
+      <c r="G27" s="54">
         <v>5</v>
       </c>
-      <c r="H27" s="57">
+      <c r="H27" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I27" s="71">
+      <c r="I27" s="63">
         <v>80995.94</v>
       </c>
-      <c r="J27" s="72">
-        <v>0</v>
-      </c>
-      <c r="K27" s="73">
+      <c r="J27" s="64">
+        <v>0</v>
+      </c>
+      <c r="K27" s="65">
         <f t="shared" si="1"/>
         <v>80995.94</v>
       </c>
-      <c r="L27" s="74">
-        <v>80995.94</v>
-      </c>
-      <c r="M27" s="75">
-        <v>0</v>
-      </c>
-      <c r="N27" s="76">
-        <f t="shared" si="2"/>
-        <v>80995.94</v>
-      </c>
-      <c r="O27" s="61">
-        <f t="shared" si="3"/>
-        <v>1.5432872314340693E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A28" s="63" t="s">
+    </row>
+    <row r="28" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A28" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="64" t="s">
+      <c r="B28" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="57">
+      <c r="D28" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="54">
         <v>5</v>
       </c>
-      <c r="F28" s="57">
+      <c r="F28" s="54">
         <v>5</v>
       </c>
-      <c r="G28" s="57">
+      <c r="G28" s="54">
         <v>5</v>
       </c>
-      <c r="H28" s="57">
+      <c r="H28" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I28" s="71">
+      <c r="I28" s="63">
         <v>103774</v>
       </c>
-      <c r="J28" s="72">
-        <v>0</v>
-      </c>
-      <c r="K28" s="73">
+      <c r="J28" s="64">
+        <v>0</v>
+      </c>
+      <c r="K28" s="65">
         <f t="shared" si="1"/>
         <v>103774</v>
       </c>
-      <c r="L28" s="74">
-        <v>103774</v>
-      </c>
-      <c r="M28" s="75">
-        <v>0</v>
-      </c>
-      <c r="N28" s="76">
-        <f t="shared" si="2"/>
-        <v>103774</v>
-      </c>
-      <c r="O28" s="61">
-        <f t="shared" si="3"/>
-        <v>1.2045406363829091E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A29" s="63" t="s">
+    </row>
+    <row r="29" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A29" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="64" t="s">
+      <c r="B29" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="64" t="s">
+      <c r="D29" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="57">
+      <c r="E29" s="54">
         <v>5</v>
       </c>
-      <c r="F29" s="57">
+      <c r="F29" s="54">
         <v>5</v>
       </c>
-      <c r="G29" s="57">
+      <c r="G29" s="54">
         <v>5</v>
       </c>
-      <c r="H29" s="57">
+      <c r="H29" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I29" s="71">
+      <c r="I29" s="63">
         <v>192349.64</v>
       </c>
-      <c r="J29" s="72">
-        <v>0</v>
-      </c>
-      <c r="K29" s="73">
+      <c r="J29" s="64">
+        <v>0</v>
+      </c>
+      <c r="K29" s="65">
         <f t="shared" si="1"/>
         <v>192349.64</v>
       </c>
-      <c r="L29" s="74">
-        <v>192349.64</v>
-      </c>
-      <c r="M29" s="75">
-        <v>0</v>
-      </c>
-      <c r="N29" s="76">
-        <f t="shared" si="2"/>
-        <v>192349.64</v>
-      </c>
-      <c r="O29" s="61">
-        <f t="shared" si="3"/>
-        <v>6.4985824772014129E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A30" s="63" t="s">
+    </row>
+    <row r="30" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A30" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="64" t="s">
+      <c r="D30" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="57">
+      <c r="E30" s="54">
         <v>5</v>
       </c>
-      <c r="F30" s="57">
+      <c r="F30" s="54">
         <v>5</v>
       </c>
-      <c r="G30" s="57">
+      <c r="G30" s="54">
         <v>5</v>
       </c>
-      <c r="H30" s="57">
+      <c r="H30" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I30" s="71">
+      <c r="I30" s="63">
         <v>1853.42</v>
       </c>
-      <c r="J30" s="72">
-        <v>0</v>
-      </c>
-      <c r="K30" s="73">
+      <c r="J30" s="64">
+        <v>0</v>
+      </c>
+      <c r="K30" s="65">
         <f t="shared" si="1"/>
         <v>1853.42</v>
       </c>
-      <c r="L30" s="74">
-        <v>1853.42</v>
-      </c>
-      <c r="M30" s="75">
-        <v>0</v>
-      </c>
-      <c r="N30" s="76">
-        <f t="shared" si="2"/>
-        <v>1853.42</v>
-      </c>
-      <c r="O30" s="61">
-        <f t="shared" si="3"/>
-        <v>6.7442889361288852E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A31" s="63" t="s">
+    </row>
+    <row r="31" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A31" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="64" t="s">
+      <c r="B31" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="64" t="s">
+      <c r="D31" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="57">
+      <c r="E31" s="54">
         <v>5</v>
       </c>
-      <c r="F31" s="57">
+      <c r="F31" s="54">
         <v>5</v>
       </c>
-      <c r="G31" s="57">
+      <c r="G31" s="54">
         <v>5</v>
       </c>
-      <c r="H31" s="57">
+      <c r="H31" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I31" s="71">
+      <c r="I31" s="63">
         <v>502208.26</v>
       </c>
-      <c r="J31" s="72">
-        <v>0</v>
-      </c>
-      <c r="K31" s="73">
+      <c r="J31" s="64">
+        <v>0</v>
+      </c>
+      <c r="K31" s="65">
         <f t="shared" si="1"/>
         <v>502208.26</v>
       </c>
-      <c r="L31" s="74">
-        <v>502208.26</v>
-      </c>
-      <c r="M31" s="75">
-        <v>0</v>
-      </c>
-      <c r="N31" s="76">
-        <f t="shared" si="2"/>
-        <v>502208.26</v>
-      </c>
-      <c r="O31" s="61">
-        <f t="shared" si="3"/>
-        <v>2.489007249701548E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="A32" s="63" t="s">
+    </row>
+    <row r="32" spans="1:11" ht="30" customHeight="1" thickBot="1">
+      <c r="A32" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="64" t="s">
+      <c r="B32" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32" s="57">
+      <c r="D32" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="54">
         <v>5</v>
       </c>
-      <c r="F32" s="57">
+      <c r="F32" s="54">
         <v>5</v>
       </c>
-      <c r="G32" s="57">
+      <c r="G32" s="54">
         <v>5</v>
       </c>
-      <c r="H32" s="57">
+      <c r="H32" s="54">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="I32" s="71">
+      <c r="I32" s="63">
         <v>96000</v>
       </c>
-      <c r="J32" s="72">
-        <v>0</v>
-      </c>
-      <c r="K32" s="73">
+      <c r="J32" s="64">
+        <v>0</v>
+      </c>
+      <c r="K32" s="65">
         <f t="shared" si="1"/>
         <v>96000</v>
       </c>
-      <c r="L32" s="74">
-        <v>96000</v>
-      </c>
-      <c r="M32" s="75">
-        <v>0</v>
-      </c>
-      <c r="N32" s="76">
-        <f t="shared" si="2"/>
-        <v>96000</v>
-      </c>
-      <c r="O32" s="61">
-        <f t="shared" si="3"/>
-        <v>1.3020833333333333E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="30" customHeight="1">
-      <c r="A33" s="63" t="s">
+    </row>
+    <row r="33" spans="1:11" ht="30" customHeight="1">
+      <c r="A33" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="64" t="s">
+      <c r="B33" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="57">
+      <c r="D33" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="54">
         <v>3</v>
       </c>
-      <c r="F33" s="57">
+      <c r="F33" s="54">
         <v>3</v>
       </c>
-      <c r="G33" s="57">
+      <c r="G33" s="54">
         <v>4</v>
       </c>
-      <c r="H33" s="57">
+      <c r="H33" s="54">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="I33" s="71">
+      <c r="I33" s="63">
         <v>404427.72</v>
       </c>
-      <c r="J33" s="72">
-        <v>0</v>
-      </c>
-      <c r="K33" s="73">
+      <c r="J33" s="64">
+        <v>0</v>
+      </c>
+      <c r="K33" s="65">
         <f t="shared" si="1"/>
         <v>404427.72</v>
       </c>
-      <c r="L33" s="74">
-        <v>404427.72</v>
-      </c>
-      <c r="M33" s="75">
-        <v>0</v>
-      </c>
-      <c r="N33" s="76">
-        <f t="shared" si="2"/>
-        <v>404427.72</v>
-      </c>
-      <c r="O33" s="61">
-        <f t="shared" si="3"/>
-        <v>8.9014669914317459E-5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="93"/>
-      <c r="B34" s="93"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
-      <c r="N34" s="93"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="76"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" s="57">
+        <f>SUMIF(J2:J33,0,H2:H33)</f>
+        <v>2146</v>
+      </c>
+      <c r="I35" s="77">
+        <f>SUM(I2:I33)</f>
+        <v>5823755.2800000003</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>